<commit_message>
added option to add name of person into output files
</commit_message>
<xml_diff>
--- a/Unti.xlsx
+++ b/Unti.xlsx
@@ -55,7 +55,7 @@
     <t xml:space="preserve">09.01.2023</t>
   </si>
   <si>
-    <t xml:space="preserve">31.01.2023</t>
+    <t xml:space="preserve">21.01.2023</t>
   </si>
 </sst>
 </file>
@@ -164,10 +164,10 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>